<commit_message>
type of tasks added
</commit_message>
<xml_diff>
--- a/E-Commerce-Dev.xlsx
+++ b/E-Commerce-Dev.xlsx
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="126">
   <si>
     <t>SL#</t>
   </si>
@@ -110,6 +110,9 @@
     <t>Rajesh Ghosh</t>
   </si>
   <si>
+    <t>Bugs</t>
+  </si>
+  <si>
     <t>T2</t>
   </si>
   <si>
@@ -122,6 +125,9 @@
     <t>José Pedro Teles</t>
   </si>
   <si>
+    <t>Exception</t>
+  </si>
+  <si>
     <t>T3</t>
   </si>
   <si>
@@ -131,6 +137,9 @@
     <t>4H</t>
   </si>
   <si>
+    <t>Improvement</t>
+  </si>
+  <si>
     <t>T4</t>
   </si>
   <si>
@@ -195,6 +204,9 @@
   </si>
   <si>
     <t>Product Category Section</t>
+  </si>
+  <si>
+    <t>Task</t>
   </si>
   <si>
     <t>T13</t>
@@ -558,8 +570,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2.0" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B4" sqref="B4" pane="bottomLeft"/>
+      <pane xSplit="3.0" ySplit="2.0" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="D1" sqref="D1" pane="topRight"/>
+      <selection activeCell="A3" sqref="A3" pane="bottomLeft"/>
+      <selection activeCell="D3" sqref="D3" pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
@@ -622,269 +636,308 @@
       <c r="G3" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="H3" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>12</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>16</v>
-      </c>
       <c r="G5" s="6" t="s">
         <v>12</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F6" s="3"/>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>12</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>12</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>12</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F11" s="3"/>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>39</v>
+        <v>42</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>39</v>
+        <v>42</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>39</v>
+        <v>42</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>39</v>
+        <v>42</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="19">
@@ -896,22 +949,25 @@
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G20" s="6" t="s">
         <v>11</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="21">
@@ -923,33 +979,36 @@
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>11</v>
       </c>
+      <c r="H22" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>10</v>
@@ -963,14 +1022,17 @@
       <c r="G23" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="H23" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>10</v>
@@ -979,44 +1041,50 @@
         <v>10</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>12</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>11</v>
       </c>
+      <c r="H25" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>12</v>
@@ -1024,229 +1092,259 @@
       <c r="G26" s="6" t="s">
         <v>11</v>
       </c>
+      <c r="H26" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="G27" s="6"/>
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G28" s="6" t="s">
         <v>12</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G29" s="6" t="s">
         <v>12</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="3" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G30" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="H30" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="I30" s="3" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>11</v>
       </c>
+      <c r="H31" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="3" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="3" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="3" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="3" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="3" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F38" s="6" t="s">
         <v>11</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="3" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>11</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="3" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>11</v>
@@ -1254,225 +1352,250 @@
       <c r="G40" s="6" t="s">
         <v>11</v>
       </c>
+      <c r="H40" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="3" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="3" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>11</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="3" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="3" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="3" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="3" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F45" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="3" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="3" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="3" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H48" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="3" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H49" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="3" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F50" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H50" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="3" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G51" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="H51" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="3" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="H52" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="55">
       <c r="D55" s="3" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="56">
       <c r="B56" s="3" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="57">
@@ -1480,7 +1603,7 @@
         <v>38.0</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="58">
@@ -1491,17 +1614,17 @@
     </row>
     <row r="59">
       <c r="D59" s="3" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="60">
       <c r="D60" s="3" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="61">
       <c r="C61" s="3" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D61">
         <f>35/5</f>

</xml_diff>

<commit_message>
data added in new columns
</commit_message>
<xml_diff>
--- a/E-Commerce-Dev.xlsx
+++ b/E-Commerce-Dev.xlsx
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="179">
   <si>
     <t>SL#</t>
   </si>
@@ -92,7 +92,7 @@
     <t>Type  of the task</t>
   </si>
   <si>
-    <t>Summery of Ticket</t>
+    <t>Summary of Ticket</t>
   </si>
   <si>
     <t>Dropdown Component</t>
@@ -122,6 +122,9 @@
     <t>(In Hours)</t>
   </si>
   <si>
+    <t>Project starts 11/6</t>
+  </si>
+  <si>
     <t>T1</t>
   </si>
   <si>
@@ -134,55 +137,97 @@
     <t>Rajesh Ghosh</t>
   </si>
   <si>
+    <t>Epic</t>
+  </si>
+  <si>
+    <t>Design and implemente the database for the project</t>
+  </si>
+  <si>
+    <t>Very High</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>Test server configaration (Local Share server)</t>
+  </si>
+  <si>
+    <t>José Pedro Teles</t>
+  </si>
+  <si>
+    <t>Exception</t>
+  </si>
+  <si>
+    <t>Configurat the server to implement</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>Preparing Deployment Environment</t>
+  </si>
+  <si>
+    <t>Improvement</t>
+  </si>
+  <si>
+    <t>Set the enviroment for people to work</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>Home page</t>
+  </si>
+  <si>
+    <t>Navbar</t>
+  </si>
+  <si>
+    <t>Login, logout, company logo, filter, categories</t>
+  </si>
+  <si>
+    <t>Web page were a user can see a log in option, the company logo, a filter option and categories from the shop</t>
+  </si>
+  <si>
+    <t>T6</t>
+  </si>
+  <si>
+    <t>Product Slider</t>
+  </si>
+  <si>
+    <t>Define Relevant Products and show each one of them after a period of time</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Rectangle in the middle of the page that displays information about featured products</t>
+  </si>
+  <si>
+    <t>T7</t>
+  </si>
+  <si>
+    <t>Blog section</t>
+  </si>
+  <si>
+    <t>Part of the Home page where people can comment and ask help to buy products</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Footer</t>
+  </si>
+  <si>
     <t>Bugs</t>
   </si>
   <si>
-    <t>T2</t>
-  </si>
-  <si>
-    <t>Test server configaration (Local Share server)</t>
-  </si>
-  <si>
-    <t>José Pedro Teles</t>
-  </si>
-  <si>
-    <t>Exception</t>
-  </si>
-  <si>
-    <t>T3</t>
-  </si>
-  <si>
-    <t>Preparing Deployment Environment</t>
-  </si>
-  <si>
-    <t>Improvement</t>
-  </si>
-  <si>
-    <t>T4</t>
-  </si>
-  <si>
-    <t>T5</t>
-  </si>
-  <si>
-    <t>Home page</t>
-  </si>
-  <si>
-    <t>Navbar</t>
-  </si>
-  <si>
-    <t>T6</t>
-  </si>
-  <si>
-    <t>Product Slider</t>
-  </si>
-  <si>
-    <t>T7</t>
-  </si>
-  <si>
-    <t>Blog section</t>
-  </si>
-  <si>
-    <t>Footer</t>
+    <t>Categories as contact us, sitemap</t>
+  </si>
+  <si>
+    <t>High</t>
   </si>
   <si>
     <t>T9</t>
@@ -200,6 +245,9 @@
     <t>Marina Camilo</t>
   </si>
   <si>
+    <t>Full Text Search Database Products</t>
+  </si>
+  <si>
     <t>T11</t>
   </si>
   <si>
@@ -209,6 +257,9 @@
     <t>Victor Padi</t>
   </si>
   <si>
+    <t>Top Selling Products carousel</t>
+  </si>
+  <si>
     <t>T12</t>
   </si>
   <si>
@@ -218,6 +269,9 @@
     <t>Task</t>
   </si>
   <si>
+    <t>Products' miniatures, adjusted by the page dimensions</t>
+  </si>
+  <si>
     <t>T13</t>
   </si>
   <si>
@@ -230,30 +284,45 @@
     <t>Product Descriptoin Section</t>
   </si>
   <si>
+    <t>Section where people can get more info about the product. How is it works? When is it recommend? How should be used? Components and benefits</t>
+  </si>
+  <si>
     <t>T15</t>
   </si>
   <si>
     <t>Buying Option / Add to cart section</t>
   </si>
   <si>
+    <t>Make sure that when you open a new page the cart is the same. If anyone is log in, it keeps the card until the user drops it. Make sure that when a product is selected is on the shopping card section. It has to be possible to change the quantity of a product</t>
+  </si>
+  <si>
     <t>T16</t>
   </si>
   <si>
     <t>Checkout and payment page</t>
   </si>
   <si>
+    <t>Get the total cost of the items of the cart in different coins. Confirm Deliver adress. Check the payment method.</t>
+  </si>
+  <si>
     <t>T18</t>
   </si>
   <si>
     <t>Blog page</t>
   </si>
   <si>
+    <t>Do a comment, change and delete user's loged in comments. See comments from other users, comment others users posts, give reactions to others user posts.</t>
+  </si>
+  <si>
     <t>T20</t>
   </si>
   <si>
     <t>Events page</t>
   </si>
   <si>
+    <t>Creat, update and delete admin's events. See next evets.</t>
+  </si>
+  <si>
     <t>T21</t>
   </si>
   <si>
@@ -263,24 +332,36 @@
     <t>Inventory Management</t>
   </si>
   <si>
+    <t>Check stock in the store. Know the last bought products and their destiny. See statics of the goods sold. Control the stock requests. Annswer the question of the clients</t>
+  </si>
+  <si>
     <t>T22</t>
   </si>
   <si>
     <t>Payment Getway integration</t>
   </si>
   <si>
+    <t>Conect to the payment portal. Check when the payment is done in the portal.</t>
+  </si>
+  <si>
     <t>T23</t>
   </si>
   <si>
     <t>Confirmation and Shipment</t>
   </si>
   <si>
+    <t>Update the status order.</t>
+  </si>
+  <si>
     <t>T24</t>
   </si>
   <si>
     <t>Coupons and offers implementation</t>
   </si>
   <si>
+    <t>Generate unique numbers of coupons. Create a section to receive any coupon or offer. Check the validation of the coupon/offer</t>
+  </si>
+  <si>
     <t>T25</t>
   </si>
   <si>
@@ -293,19 +374,25 @@
     <t>Admin Login and Registration</t>
   </si>
   <si>
+    <t>Login should be visible during the site movimentation. Form for registration with name, last name, email and password. Add to the database the ew user.</t>
+  </si>
+  <si>
     <t>T27</t>
   </si>
   <si>
     <t>Product Upload implementation</t>
   </si>
   <si>
+    <t>Form with description, image, cost, and extra information sections. Add to the database the new poduct. It should be visible to users after filling the form</t>
+  </si>
+  <si>
     <t>T28</t>
   </si>
   <si>
     <t xml:space="preserve">Offer and product update </t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>Form with description, image, cost, and extra information sections. Update the database about the existing poduct. It should be visible to users after filling the form.</t>
   </si>
   <si>
     <t>T29</t>
@@ -314,6 +401,9 @@
     <t>Admin Logout</t>
   </si>
   <si>
+    <t>After closing the browser or click a botton, the admin account should be unacessible</t>
+  </si>
+  <si>
     <t>T30</t>
   </si>
   <si>
@@ -332,42 +422,63 @@
     <t>User Login and Logout</t>
   </si>
   <si>
+    <t xml:space="preserve">Login should be visible during the site movimentation. Ater click the logout botton or close the browser the user account should be unacessible </t>
+  </si>
+  <si>
     <t>T34</t>
   </si>
   <si>
     <t>User Registration</t>
   </si>
   <si>
+    <t>Form for reistration with name last name, email and password. Add to the database the ew user.</t>
+  </si>
+  <si>
     <t>T35</t>
   </si>
   <si>
     <t>Report Problem System</t>
   </si>
   <si>
+    <t>Form with type of question, and a descrition section. When submited it should be attached the client ID and the name of the user.</t>
+  </si>
+  <si>
     <t>T36</t>
   </si>
   <si>
     <t>Set Profile</t>
   </si>
   <si>
+    <t>Add a image to the account. Also, define the addres of the user</t>
+  </si>
+  <si>
     <t>T37</t>
   </si>
   <si>
     <t>Update Profile</t>
   </si>
   <si>
+    <t>Form whereit should be possible to change the password, adress and image</t>
+  </si>
+  <si>
     <t>T38</t>
   </si>
   <si>
     <t>My Orders Section</t>
   </si>
   <si>
+    <t>List the orders that the user already had</t>
+  </si>
+  <si>
     <t>T39</t>
   </si>
   <si>
     <t>Description of Order Section</t>
   </si>
   <si>
+    <t xml:space="preserve">Show the product list of the order that user seected </t>
+  </si>
+  <si>
     <t>T40</t>
   </si>
   <si>
@@ -383,12 +494,18 @@
     <t>Form to send message Section</t>
   </si>
   <si>
+    <t>Form with name, email, and description area.</t>
+  </si>
+  <si>
     <t>T43</t>
   </si>
   <si>
     <t>Formal contacts Section with map</t>
   </si>
   <si>
+    <t>Map with the address of the store. Email and phone of the store</t>
+  </si>
+  <si>
     <t>T44</t>
   </si>
   <si>
@@ -401,34 +518,55 @@
     <t>Testing Shopping Cart</t>
   </si>
   <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Test if we the product selected is in the shopping cart. Check if the shopping cart is the same when I log in in a different enviroment</t>
+  </si>
+  <si>
     <t>T46</t>
   </si>
   <si>
     <t>Search Form, Sorting, Filtering, Pagination</t>
   </si>
   <si>
+    <t>Test if the Full Text Searching is working as it should be</t>
+  </si>
+  <si>
     <t>T47</t>
   </si>
   <si>
     <t>Create account and Login Test</t>
   </si>
   <si>
+    <t>Create account, and see if it is succefully loged in. Also check if we restart the browser we need to log in again</t>
+  </si>
+  <si>
     <t>T48</t>
   </si>
   <si>
     <t>Payments</t>
   </si>
   <si>
+    <t>Check if the payment section knows if the payment is already done</t>
+  </si>
+  <si>
     <t>T49</t>
   </si>
   <si>
     <t>Post Purchase Test</t>
   </si>
   <si>
+    <t>Check if user can purchase products.</t>
+  </si>
+  <si>
     <t>T50</t>
   </si>
   <si>
     <t>Go Live / Deployment</t>
+  </si>
+  <si>
+    <t>Prepare server to receive a bigger amount of requests and lauch a version of the product</t>
   </si>
   <si>
     <t>Total Time:</t>
@@ -474,6 +612,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="M/d/yyyy"/>
+    <numFmt numFmtId="165" formatCode="m/d"/>
+    <numFmt numFmtId="166" formatCode="m-d"/>
+  </numFmts>
   <fonts count="9">
     <font>
       <sz val="10.0"/>
@@ -556,7 +699,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -581,14 +724,29 @@
     <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
@@ -787,11 +945,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1489547280"/>
-        <c:axId val="1691937077"/>
+        <c:axId val="1305043545"/>
+        <c:axId val="743746004"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1489547280"/>
+        <c:axId val="1305043545"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -823,10 +981,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1691937077"/>
+        <c:crossAx val="743746004"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1691937077"/>
+        <c:axId val="743746004"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -857,7 +1015,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1489547280"/>
+        <c:crossAx val="1305043545"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1037,11 +1195,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="466646604"/>
-        <c:axId val="1746407028"/>
+        <c:axId val="2104878673"/>
+        <c:axId val="1367673364"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="466646604"/>
+        <c:axId val="2104878673"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1056,10 +1214,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1746407028"/>
+        <c:crossAx val="1367673364"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1746407028"/>
+        <c:axId val="1367673364"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1090,7 +1248,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="466646604"/>
+        <c:crossAx val="2104878673"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1234,10 +1392,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3.0" ySplit="2.0" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="D1" sqref="D1" pane="topRight"/>
+      <pane xSplit="2.0" ySplit="2.0" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="C1" sqref="C1" pane="topRight"/>
       <selection activeCell="A3" sqref="A3" pane="bottomLeft"/>
-      <selection activeCell="D3" sqref="D3" pane="bottomRight"/>
+      <selection activeCell="C3" sqref="C3" pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
@@ -1250,11 +1408,11 @@
     <col customWidth="1" min="7" max="8" width="18.71"/>
     <col customWidth="1" min="9" max="9" width="25.86"/>
     <col customWidth="1" min="10" max="10" width="27.14"/>
-    <col customWidth="1" min="11" max="11" width="16.0"/>
-    <col customWidth="1" min="12" max="12" width="17.86"/>
+    <col customWidth="1" hidden="1" min="11" max="11" width="21.14"/>
+    <col customWidth="1" hidden="1" min="12" max="12" width="17.86"/>
     <col customWidth="1" min="13" max="13" width="21.71"/>
     <col customWidth="1" min="14" max="14" width="24.29"/>
-    <col customWidth="1" min="15" max="15" width="20.71"/>
+    <col customWidth="1" min="15" max="15" width="41.71"/>
     <col customWidth="1" min="16" max="16" width="20.0"/>
   </cols>
   <sheetData>
@@ -1317,13 +1475,16 @@
       <c r="E2" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="L2" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D3" s="4">
         <v>16.0</v>
@@ -1332,21 +1493,36 @@
         <v>5.0</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="9">
+        <v>43047.0</v>
+      </c>
+      <c r="M3" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N3" s="4">
+        <v>0.1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D4" s="4">
         <v>5.0</v>
@@ -1355,21 +1531,37 @@
         <v>2.0</v>
       </c>
       <c r="F4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="10"/>
+      <c r="K4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>25</v>
+      <c r="L4" s="9">
+        <v>43045.0</v>
+      </c>
+      <c r="M4" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N4" s="4">
+        <v>0.2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D5" s="4">
         <v>4.0</v>
@@ -1378,30 +1570,48 @@
         <v>0.0</v>
       </c>
       <c r="F5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" s="11"/>
+      <c r="K5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>28</v>
+      <c r="L5" s="9">
+        <v>43046.0</v>
+      </c>
+      <c r="M5" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N5" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F6" s="4"/>
+      <c r="I6" s="12"/>
+      <c r="L6" s="9"/>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D7" s="4">
         <v>6.0</v>
@@ -1410,21 +1620,40 @@
         <v>4.0</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" s="11"/>
+      <c r="K7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" s="9">
+        <v>43046.0</v>
+      </c>
+      <c r="M7" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N7" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="O7" s="13" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D8" s="4">
         <v>8.0</v>
@@ -1433,21 +1662,40 @@
         <v>2.0</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" s="11"/>
+      <c r="K8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L8" s="9">
+        <v>43053.0</v>
+      </c>
+      <c r="M8" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N8" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="O8" s="8" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D9" s="4">
         <v>5.0</v>
@@ -1456,19 +1704,35 @@
         <v>1.0</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="J9" s="11"/>
+      <c r="K9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="L9" s="9">
+        <v>43054.0</v>
+      </c>
+      <c r="M9" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N9" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4"/>
       <c r="C10" s="4" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="D10" s="4">
         <v>5.0</v>
@@ -1477,30 +1741,48 @@
         <v>2.0</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>21</v>
+        <v>50</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="J10" s="11"/>
+      <c r="K10" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L10" s="9">
+        <v>43048.0</v>
+      </c>
+      <c r="M10" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N10" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="F11" s="4"/>
+      <c r="I11" s="12"/>
+      <c r="L11" s="9"/>
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>40</v>
+        <v>54</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>55</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="D12" s="4">
         <v>12.0</v>
@@ -1509,21 +1791,37 @@
         <v>15.0</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="J12" s="11"/>
+      <c r="K12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L12" s="9">
+        <v>43048.0</v>
+      </c>
+      <c r="M12" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N12" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="D13" s="4">
         <v>5.0</v>
@@ -1532,21 +1830,36 @@
         <v>5.0</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>45</v>
+        <v>57</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>61</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L13" s="9">
+        <v>43049.0</v>
+      </c>
+      <c r="M13" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N13" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="D14" s="4">
         <v>8.0</v>
@@ -1555,29 +1868,46 @@
         <v>8.0</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>45</v>
+        <v>57</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>61</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>48</v>
+        <v>65</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L14" s="9">
+        <v>43052.0</v>
+      </c>
+      <c r="M14" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N14" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>49</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="I15" s="12"/>
+      <c r="L15" s="9"/>
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="D16" s="4">
         <v>4.0</v>
@@ -1585,22 +1915,37 @@
       <c r="E16" s="4">
         <v>4.0</v>
       </c>
-      <c r="F16" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>45</v>
+      <c r="F16" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>61</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>48</v>
+        <v>65</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L16" s="9">
+        <v>43048.0</v>
+      </c>
+      <c r="M16" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N16" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="D17" s="4">
         <v>8.0</v>
@@ -1608,22 +1953,37 @@
       <c r="E17" s="4">
         <v>8.0</v>
       </c>
-      <c r="F17" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>45</v>
+      <c r="F17" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>61</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>48</v>
+        <v>65</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L17" s="9">
+        <v>43047.0</v>
+      </c>
+      <c r="M17" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N17" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="D18" s="4">
         <v>3.0</v>
@@ -1631,14 +1991,29 @@
       <c r="E18" s="4">
         <v>3.0</v>
       </c>
-      <c r="F18" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>45</v>
+      <c r="F18" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>61</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>21</v>
+        <v>50</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L18" s="9">
+        <v>43048.0</v>
+      </c>
+      <c r="M18" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N18" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="19">
@@ -1647,13 +2022,15 @@
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
+      <c r="I19" s="12"/>
+      <c r="L19" s="9"/>
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="D20" s="4">
         <v>8.0</v>
@@ -1662,13 +2039,28 @@
         <v>8.0</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="L20" s="9">
+        <v>43055.0</v>
+      </c>
+      <c r="M20" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N20" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="21">
@@ -1677,13 +2069,15 @@
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
+      <c r="I21" s="12"/>
+      <c r="L21" s="9"/>
     </row>
     <row r="22">
       <c r="A22" s="4" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="D22" s="4">
         <v>8.0</v>
@@ -1692,24 +2086,39 @@
         <v>8.0</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H22" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="K22" s="4" t="s">
         <v>48</v>
+      </c>
+      <c r="L22" s="9">
+        <v>43053.0</v>
+      </c>
+      <c r="M22" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N22" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="4" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="D23" s="4">
         <v>16.0</v>
@@ -1718,22 +2127,37 @@
         <v>16.0</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>48</v>
+        <v>65</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L23" s="9">
+        <v>43049.0</v>
+      </c>
+      <c r="M23" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N23" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="4" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="D24" s="4">
         <v>16.0</v>
@@ -1742,21 +2166,36 @@
         <v>16.0</v>
       </c>
       <c r="F24" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="K24" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G24" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>28</v>
+      <c r="L24" s="9">
+        <v>43048.0</v>
+      </c>
+      <c r="M24" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N24" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="4" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="D25" s="4">
         <v>5.0</v>
@@ -1765,21 +2204,36 @@
         <v>5.0</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>48</v>
+        <v>65</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L25" s="9">
+        <v>43046.0</v>
+      </c>
+      <c r="M25" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N25" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="4" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="D26" s="4">
         <v>8.0</v>
@@ -1788,30 +2242,47 @@
         <v>8.0</v>
       </c>
       <c r="F26" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G26" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G26" s="7" t="s">
-        <v>19</v>
-      </c>
       <c r="H26" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="K26" s="4" t="s">
         <v>48</v>
+      </c>
+      <c r="L26" s="9">
+        <v>43054.0</v>
+      </c>
+      <c r="M26" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N26" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="4" t="s">
-        <v>70</v>
+        <v>97</v>
       </c>
       <c r="G27" s="7"/>
+      <c r="I27" s="12"/>
+      <c r="L27" s="9"/>
     </row>
     <row r="28">
       <c r="A28" s="4" t="s">
-        <v>71</v>
+        <v>98</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="D28" s="4">
         <v>8.0</v>
@@ -1820,21 +2291,36 @@
         <v>8.0</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>21</v>
+        <v>50</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L28" s="9">
+        <v>43052.0</v>
+      </c>
+      <c r="M28" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N28" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="4" t="s">
-        <v>74</v>
+        <v>102</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>75</v>
+        <v>103</v>
       </c>
       <c r="D29" s="4">
         <v>11.0</v>
@@ -1842,22 +2328,37 @@
       <c r="E29" s="4">
         <v>11.0</v>
       </c>
-      <c r="F29" s="9" t="s">
-        <v>45</v>
+      <c r="F29" s="15" t="s">
+        <v>61</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>21</v>
+        <v>50</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L29" s="9">
+        <v>43052.0</v>
+      </c>
+      <c r="M29" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N29" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="4" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="D30" s="4">
         <v>5.0</v>
@@ -1865,25 +2366,37 @@
       <c r="E30" s="4">
         <v>5.0</v>
       </c>
-      <c r="F30" s="9" t="s">
-        <v>45</v>
+      <c r="F30" s="15" t="s">
+        <v>61</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>78</v>
+        <v>50</v>
+      </c>
+      <c r="I30" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L30" s="9">
+        <v>43053.0</v>
+      </c>
+      <c r="M30" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N30" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="4" t="s">
-        <v>79</v>
+        <v>108</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="D31" s="4">
         <v>3.0</v>
@@ -1891,40 +2404,61 @@
       <c r="E31" s="4">
         <v>3.0</v>
       </c>
-      <c r="F31" s="9" t="s">
-        <v>45</v>
+      <c r="F31" s="15" t="s">
+        <v>61</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H31" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="K31" s="4" t="s">
         <v>48</v>
+      </c>
+      <c r="L31" s="9">
+        <v>43055.0</v>
+      </c>
+      <c r="M31" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N31" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="4" t="s">
-        <v>81</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="I32" s="12"/>
+      <c r="L32" s="9"/>
     </row>
     <row r="33">
       <c r="A33" s="4" t="s">
-        <v>82</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="I33" s="12"/>
+      <c r="L33" s="9"/>
     </row>
     <row r="34">
       <c r="A34" s="4" t="s">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>84</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="I34" s="12"/>
+      <c r="L34" s="9"/>
     </row>
     <row r="35">
       <c r="A35" s="4" t="s">
-        <v>85</v>
+        <v>115</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="D35" s="4">
         <v>4.0</v>
@@ -1933,21 +2467,36 @@
         <v>4.0</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>48</v>
+        <v>65</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L35" s="9">
+        <v>43049.0</v>
+      </c>
+      <c r="M35" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N35" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="4" t="s">
-        <v>87</v>
+        <v>118</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>88</v>
+        <v>119</v>
       </c>
       <c r="D36" s="4">
         <v>6.0</v>
@@ -1956,21 +2505,36 @@
         <v>6.0</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>48</v>
+        <v>65</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="K36" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L36" s="9">
+        <v>43052.0</v>
+      </c>
+      <c r="M36" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N36" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="4" t="s">
-        <v>89</v>
+        <v>121</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>90</v>
+        <v>122</v>
       </c>
       <c r="D37" s="4">
         <v>4.0</v>
@@ -1979,21 +2543,36 @@
         <v>4.0</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="H37" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="K37" s="4" t="s">
         <v>48</v>
+      </c>
+      <c r="L37" s="9">
+        <v>43054.0</v>
+      </c>
+      <c r="M37" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N37" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="4" t="s">
-        <v>91</v>
+        <v>124</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>92</v>
+        <v>125</v>
       </c>
       <c r="D38" s="4">
         <v>8.0</v>
@@ -2002,21 +2581,36 @@
         <v>8.0</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
+      </c>
+      <c r="I38" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="K38" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L38" s="9">
+        <v>43052.0</v>
+      </c>
+      <c r="M38" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N38" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="4" t="s">
-        <v>93</v>
+        <v>127</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="D39" s="4">
         <v>4.0</v>
@@ -2025,21 +2619,36 @@
         <v>4.0</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
+      </c>
+      <c r="I39" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L39" s="9">
+        <v>43053.0</v>
+      </c>
+      <c r="M39" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N39" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="4" t="s">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>96</v>
+        <v>131</v>
       </c>
       <c r="D40" s="4">
         <v>3.0</v>
@@ -2048,22 +2657,37 @@
         <v>3.0</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>48</v>
+        <v>65</v>
+      </c>
+      <c r="I40" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="K40" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L40" s="9">
+        <v>43054.0</v>
+      </c>
+      <c r="M40" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N40" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="4" t="s">
-        <v>97</v>
+        <v>133</v>
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="4" t="s">
-        <v>98</v>
+        <v>134</v>
       </c>
       <c r="D41" s="4">
         <v>3.0</v>
@@ -2072,34 +2696,53 @@
         <v>3.0</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
+      </c>
+      <c r="I41" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="K41" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L41" s="9">
+        <v>43054.0</v>
+      </c>
+      <c r="M41" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N41" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="4" t="s">
-        <v>99</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="I42" s="12"/>
+      <c r="L42" s="9"/>
     </row>
     <row r="43">
       <c r="A43" s="4" t="s">
-        <v>100</v>
+        <v>137</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>101</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="I43" s="12"/>
+      <c r="L43" s="9"/>
     </row>
     <row r="44">
       <c r="A44" s="4" t="s">
-        <v>102</v>
+        <v>139</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>103</v>
+        <v>140</v>
       </c>
       <c r="D44" s="4">
         <v>5.0</v>
@@ -2108,21 +2751,36 @@
         <v>5.0</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
+      </c>
+      <c r="I44" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="K44" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="L44" s="9">
+        <v>43055.0</v>
+      </c>
+      <c r="M44" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N44" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="4" t="s">
-        <v>104</v>
+        <v>142</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>105</v>
+        <v>143</v>
       </c>
       <c r="D45" s="4">
         <v>4.0</v>
@@ -2131,29 +2789,47 @@
         <v>4.0</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G45" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I45" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="K45" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H45" s="4" t="s">
-        <v>48</v>
+      <c r="L45" s="9">
+        <v>43047.0</v>
+      </c>
+      <c r="M45" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N45" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="4" t="s">
-        <v>106</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="I46" s="12"/>
+      <c r="L46" s="9"/>
+      <c r="M46" s="4"/>
     </row>
     <row r="47">
       <c r="A47" s="4" t="s">
-        <v>107</v>
+        <v>146</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>108</v>
+        <v>147</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>109</v>
+        <v>148</v>
       </c>
       <c r="D47" s="4">
         <v>6.0</v>
@@ -2162,21 +2838,36 @@
         <v>6.0</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>21</v>
+        <v>149</v>
+      </c>
+      <c r="I47" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="K47" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L47" s="9">
+        <v>43053.0</v>
+      </c>
+      <c r="M47" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N47" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C48" s="10" t="s">
-        <v>111</v>
+        <v>151</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>152</v>
       </c>
       <c r="D48" s="4">
         <v>8.0</v>
@@ -2185,21 +2876,36 @@
         <v>8.0</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>21</v>
+        <v>149</v>
+      </c>
+      <c r="I48" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="K48" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L48" s="9">
+        <v>43054.0</v>
+      </c>
+      <c r="M48" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N48" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="4" t="s">
-        <v>112</v>
+        <v>154</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>113</v>
+        <v>155</v>
       </c>
       <c r="D49" s="4">
         <v>6.0</v>
@@ -2207,22 +2913,37 @@
       <c r="E49" s="4">
         <v>6.0</v>
       </c>
-      <c r="F49" s="9" t="s">
-        <v>45</v>
+      <c r="F49" s="15" t="s">
+        <v>61</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>21</v>
+        <v>149</v>
+      </c>
+      <c r="I49" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="K49" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L49" s="9">
+        <v>43055.0</v>
+      </c>
+      <c r="M49" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N49" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="4" t="s">
-        <v>114</v>
+        <v>157</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>115</v>
+        <v>158</v>
       </c>
       <c r="D50" s="4">
         <v>3.0</v>
@@ -2231,21 +2952,36 @@
         <v>3.0</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>21</v>
+        <v>149</v>
+      </c>
+      <c r="I50" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="K50" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L50" s="9">
+        <v>43053.0</v>
+      </c>
+      <c r="M50" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N50" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="4" t="s">
-        <v>116</v>
+        <v>160</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>117</v>
+        <v>161</v>
       </c>
       <c r="D51" s="4">
         <v>4.0</v>
@@ -2254,21 +2990,36 @@
         <v>4.0</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G51" s="9" t="s">
-        <v>45</v>
+        <v>57</v>
+      </c>
+      <c r="G51" s="15" t="s">
+        <v>61</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>21</v>
+        <v>149</v>
+      </c>
+      <c r="I51" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="K51" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L51" s="9">
+        <v>43054.0</v>
+      </c>
+      <c r="M51" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N51" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="4" t="s">
-        <v>118</v>
+        <v>163</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>119</v>
+        <v>164</v>
       </c>
       <c r="D52" s="4">
         <v>4.0</v>
@@ -2277,26 +3028,44 @@
         <v>4.0</v>
       </c>
       <c r="F52" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G52" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I52" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="K52" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G52" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H52" s="4" t="s">
-        <v>48</v>
-      </c>
+      <c r="L52" s="9">
+        <v>43056.0</v>
+      </c>
+      <c r="M52" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N52" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="M53" s="4"/>
     </row>
     <row r="55">
       <c r="D55" s="4" t="s">
-        <v>120</v>
+        <v>166</v>
       </c>
     </row>
     <row r="56">
       <c r="B56" s="4" t="s">
-        <v>121</v>
+        <v>167</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>122</v>
+        <v>168</v>
       </c>
     </row>
     <row r="57">
@@ -2304,7 +3073,7 @@
         <v>38.0</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>123</v>
+        <v>169</v>
       </c>
     </row>
     <row r="58">
@@ -2315,17 +3084,17 @@
     </row>
     <row r="59">
       <c r="D59" s="4" t="s">
-        <v>124</v>
+        <v>170</v>
       </c>
     </row>
     <row r="60">
       <c r="D60" s="4" t="s">
-        <v>125</v>
+        <v>171</v>
       </c>
     </row>
     <row r="61">
       <c r="C61" s="4" t="s">
-        <v>126</v>
+        <v>172</v>
       </c>
       <c r="D61">
         <f>35/5</f>
@@ -2350,184 +3119,184 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>127</v>
+        <v>173</v>
       </c>
       <c r="B1">
         <f>sum(Sheet1!D3:D52)</f>
         <v>249</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>128</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="13">
+      <c r="A3" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="18">
         <f>COUNTIF(Sheet1!$G$3:$G$52,A3)</f>
         <v>8</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="13">
+      <c r="A4" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="18">
         <f>COUNTIF(Sheet1!$G$3:$G$52,A4)</f>
         <v>7</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="13">
+      <c r="A5" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="18">
         <f>COUNTIF(Sheet1!$G$3:$G$52,A5)</f>
         <v>6</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="13">
+      <c r="A6" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="18">
         <f>COUNTIF(Sheet1!$G$3:$G$52,A6)</f>
         <v>12</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="13">
+      <c r="A7" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="18">
         <f>COUNTIF(Sheet1!$G$3:$G$52,A7)</f>
         <v>5</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="11" t="s">
-        <v>129</v>
+      <c r="A9" s="16" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>131</v>
+      <c r="A10" s="19"/>
+      <c r="B10" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="13">
+      <c r="A11" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="18">
         <f>COUNTIF(Sheet1!$F$3:$F$52,A11)</f>
         <v>8</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="17">
         <f>SUMIF(Sheet1!$F$3:$F$52,A11,Sheet1!$D$3:$D$52)</f>
         <v>51</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="13">
+      <c r="A12" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="18">
         <f>COUNTIF(Sheet1!$F$3:$F$52,A12)</f>
         <v>8</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="17">
         <f>SUMIF(Sheet1!$F$3:$F$52,A12,Sheet1!$D$3:$D$52)</f>
         <v>48</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="13">
+      <c r="A13" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="18">
         <f>COUNTIF(Sheet1!$F$3:$F$52,A13)</f>
         <v>6</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="17">
         <f>SUMIF(Sheet1!$F$3:$F$52,A13,Sheet1!$D$3:$D$52)</f>
         <v>50</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="13">
+      <c r="A14" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="18">
         <f>COUNTIF(Sheet1!$F$3:$F$52,A14)</f>
         <v>9</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="17">
         <f>SUMIF(Sheet1!$F$3:$F$52,A14,Sheet1!$D$3:$D$52)</f>
         <v>52</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="13">
+      <c r="A15" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="18">
         <f>COUNTIF(Sheet1!$F$3:$F$52,A15)</f>
         <v>7</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="17">
         <f>SUMIF(Sheet1!$F$3:$F$52,A15,Sheet1!$D$3:$D$52)</f>
         <v>48</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="11" t="s">
-        <v>132</v>
+      <c r="A17" s="16" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="13">
+      <c r="A18" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="18">
         <f>COUNTIF(Sheet1!$H$3:$H$52,A18)</f>
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="13">
+      <c r="A19" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="18">
         <f>COUNTIF(Sheet1!$H$3:$H$52,A19)</f>
         <v>2</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="13">
+      <c r="A20" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="18">
         <f>COUNTIF(Sheet1!$H$3:$H$52,A20)</f>
         <v>11</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="13">
+      <c r="A21" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="18">
         <f>COUNTIF(Sheet1!$H$3:$H$52,A21)</f>
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23">

</xml_diff>

<commit_message>
dropdown added and fixed the component
</commit_message>
<xml_diff>
--- a/E-Commerce-Dev.xlsx
+++ b/E-Commerce-Dev.xlsx
@@ -4,7 +4,8 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="Dashboard" sheetId="2" r:id="rId4"/>
+    <sheet state="visible" name="Dropdown Lists" sheetId="2" r:id="rId4"/>
+    <sheet state="visible" name="Dashboard" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -58,43 +59,178 @@
 	-Rajesh Ghosh</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C30">
-      <text>
-        <t xml:space="preserve">Is this CRUD?(creat, update and delete?)
-	-Pedro Teles</t>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="213">
+  <si>
+    <t>Team Members:</t>
+  </si>
   <si>
     <t>SL#</t>
   </si>
   <si>
+    <t>Type of the Task:</t>
+  </si>
+  <si>
+    <t>Type of Component:</t>
+  </si>
+  <si>
+    <t>Type of Priority:</t>
+  </si>
+  <si>
+    <t>Fix Version:</t>
+  </si>
+  <si>
+    <t>Environment:</t>
+  </si>
+  <si>
+    <t>Cansu Salkıç</t>
+  </si>
+  <si>
     <t>TASK</t>
   </si>
   <si>
+    <t>Bug</t>
+  </si>
+  <si>
     <t>ORIGINAL ESTIMATION</t>
   </si>
   <si>
+    <t>Data Base</t>
+  </si>
+  <si>
+    <t>Very High</t>
+  </si>
+  <si>
+    <t>1.0.0.0</t>
+  </si>
+  <si>
+    <t>Production</t>
+  </si>
+  <si>
+    <t>José Pedro Teles</t>
+  </si>
+  <si>
+    <t>Improvement</t>
+  </si>
+  <si>
+    <t>Backend</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Deployment</t>
+  </si>
+  <si>
+    <t>Rajesh Ghosh</t>
+  </si>
+  <si>
+    <t>Epic</t>
+  </si>
+  <si>
+    <t>Backend,Shopping</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Marina Camilo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing </t>
+  </si>
+  <si>
+    <t>Home Page</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Stage</t>
+  </si>
+  <si>
     <t>REMAINING ESTIMATION</t>
   </si>
   <si>
+    <t>Victor Padi</t>
+  </si>
+  <si>
     <t xml:space="preserve">Assigne </t>
   </si>
   <si>
+    <t>UI</t>
+  </si>
+  <si>
     <t>Reporter</t>
   </si>
   <si>
+    <t>Home Page,Data Base</t>
+  </si>
+  <si>
+    <t>Exception</t>
+  </si>
+  <si>
+    <t>Home Page,Blog Page</t>
+  </si>
+  <si>
+    <t>Data Issue</t>
+  </si>
+  <si>
+    <t>Producs Page</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Produtos Page,Data Base</t>
+  </si>
+  <si>
+    <t>Product Page,Shopping</t>
+  </si>
+  <si>
+    <t>Blog Page,Data Base</t>
+  </si>
+  <si>
+    <t>Events Page,Data Base</t>
+  </si>
+  <si>
+    <t>Admin,Data Base</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Admin,User</t>
+  </si>
+  <si>
+    <t>User,Data Base</t>
+  </si>
+  <si>
+    <t>User,Shopping</t>
+  </si>
+  <si>
+    <t>User,Data Base,Shopping</t>
+  </si>
+  <si>
     <t>Type  of the task</t>
   </si>
   <si>
+    <t>Contact Us</t>
+  </si>
+  <si>
     <t>Summary of Ticket</t>
   </si>
   <si>
+    <t>Shopping</t>
+  </si>
+  <si>
     <t>Dropdown Component</t>
   </si>
   <si>
@@ -131,19 +267,12 @@
     <t>Database design</t>
   </si>
   <si>
-    <t>Cansu Salkıç</t>
-  </si>
-  <si>
-    <t>Rajesh Ghosh</t>
-  </si>
-  <si>
-    <t>Epic</t>
-  </si>
-  <si>
     <t>Design and implemente the database for the project</t>
   </si>
   <si>
-    <t>Very High</t>
+    <t>1. Design Database
+2. Create Database
+3. Imlplement Database</t>
   </si>
   <si>
     <t>T2</t>
@@ -152,12 +281,6 @@
     <t>Test server configaration (Local Share server)</t>
   </si>
   <si>
-    <t>José Pedro Teles</t>
-  </si>
-  <si>
-    <t>Exception</t>
-  </si>
-  <si>
     <t>Configurat the server to implement</t>
   </si>
   <si>
@@ -167,9 +290,6 @@
     <t>Preparing Deployment Environment</t>
   </si>
   <si>
-    <t>Improvement</t>
-  </si>
-  <si>
     <t>Set the enviroment for people to work</t>
   </si>
   <si>
@@ -200,9 +320,6 @@
     <t>Define Relevant Products and show each one of them after a period of time</t>
   </si>
   <si>
-    <t>Medium</t>
-  </si>
-  <si>
     <t>Rectangle in the middle of the page that displays information about featured products</t>
   </si>
   <si>
@@ -215,407 +332,387 @@
     <t>Part of the Home page where people can comment and ask help to buy products</t>
   </si>
   <si>
-    <t>Low</t>
-  </si>
-  <si>
     <t>Footer</t>
   </si>
   <si>
+    <t>Categories as contact us, sitemap</t>
+  </si>
+  <si>
+    <t>T9</t>
+  </si>
+  <si>
+    <t>T10</t>
+  </si>
+  <si>
+    <t>Product Page</t>
+  </si>
+  <si>
+    <t>Filtering Option / Serach Product</t>
+  </si>
+  <si>
+    <t>Full Text Search Database Products</t>
+  </si>
+  <si>
+    <t>T11</t>
+  </si>
+  <si>
+    <t>Top Selling Produc Slider</t>
+  </si>
+  <si>
+    <t>Top Selling Products carousel</t>
+  </si>
+  <si>
+    <t>T12</t>
+  </si>
+  <si>
+    <t>Product Category Section</t>
+  </si>
+  <si>
+    <t>Products' miniatures, adjusted by the page dimensions</t>
+  </si>
+  <si>
+    <t>T13</t>
+  </si>
+  <si>
+    <t>T14</t>
+  </si>
+  <si>
+    <t>About Product Page</t>
+  </si>
+  <si>
+    <t>Product Descriptoin Section</t>
+  </si>
+  <si>
+    <t>Section where people can get more info about the product. How is it works? When is it recommend? How should be used? Components and benefits</t>
+  </si>
+  <si>
+    <t>T15</t>
+  </si>
+  <si>
+    <t>Buying Option / Add to cart section</t>
+  </si>
+  <si>
+    <t>Make sure that when you open a new page the cart is the same. If anyone is log in, it keeps the card until the user drops it. Make sure that when a product is selected is on the shopping card section. It has to be possible to change the quantity of a product</t>
+  </si>
+  <si>
+    <t>T16</t>
+  </si>
+  <si>
+    <t>Checkout and payment page</t>
+  </si>
+  <si>
+    <t>Get the total cost of the items of the cart in different coins. Confirm Deliver adress. Check the payment method.</t>
+  </si>
+  <si>
+    <t>T18</t>
+  </si>
+  <si>
+    <t>Blog page</t>
+  </si>
+  <si>
+    <t>Do a comment, change and delete user's loged in comments. See comments from other users, comment others users posts, give reactions to others user posts.</t>
+  </si>
+  <si>
+    <t>T20</t>
+  </si>
+  <si>
+    <t>Events page</t>
+  </si>
+  <si>
+    <t>Creat, update and delete admin's events. See next evets.</t>
+  </si>
+  <si>
+    <t>T21</t>
+  </si>
+  <si>
+    <t>Ecommerce Features</t>
+  </si>
+  <si>
+    <t>Inventory Management</t>
+  </si>
+  <si>
+    <t>Check stock in the store. Know the last bought products and their destiny. See statics of the goods sold. Control the stock requests. Annswer the question of the clients</t>
+  </si>
+  <si>
+    <t>T22</t>
+  </si>
+  <si>
+    <t>Payment Gateway integration</t>
+  </si>
+  <si>
+    <t>Conect to the payment portal. Check when the payment is done in the portal.</t>
+  </si>
+  <si>
+    <t>T23</t>
+  </si>
+  <si>
+    <t>Confirmation and Shipment</t>
+  </si>
+  <si>
+    <t>Update the status order.</t>
+  </si>
+  <si>
+    <t>T24</t>
+  </si>
+  <si>
+    <t>Coupons and offers implementation</t>
+  </si>
+  <si>
+    <t>Generate unique numbers of coupons. Create a section to receive any coupon or offer. Check the validation of the coupon/offer</t>
+  </si>
+  <si>
+    <t>T25</t>
+  </si>
+  <si>
+    <t>T26</t>
+  </si>
+  <si>
+    <t>Admin Panel</t>
+  </si>
+  <si>
+    <t>Admin Login and Registration</t>
+  </si>
+  <si>
+    <t>Login should be visible during the site movimentation. Form for registration with name, last name, email and password. Add to the database the ew user.</t>
+  </si>
+  <si>
+    <t>T27</t>
+  </si>
+  <si>
+    <t>Product Upload implementation</t>
+  </si>
+  <si>
+    <t>Form with description, image, cost, and extra information sections. Add to the database the new poduct. It should be visible to users after filling the form</t>
+  </si>
+  <si>
+    <t>T28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offer and product update </t>
+  </si>
+  <si>
+    <t>Form with description, image, cost, and extra information sections. Update the database about the existing poduct. It should be visible to users after filling the form.</t>
+  </si>
+  <si>
+    <t>T29</t>
+  </si>
+  <si>
+    <t>Admin Logout</t>
+  </si>
+  <si>
+    <t>After closing the browser or click a botton, the admin account should be unacessible</t>
+  </si>
+  <si>
+    <t>T30</t>
+  </si>
+  <si>
+    <t>T31</t>
+  </si>
+  <si>
+    <t>T32</t>
+  </si>
+  <si>
+    <t>User Page</t>
+  </si>
+  <si>
+    <t>T33</t>
+  </si>
+  <si>
+    <t>User Login and Logout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login should be visible during the site movimentation. Ater click the logout botton or close the browser the user account should be unacessible </t>
+  </si>
+  <si>
+    <t>T34</t>
+  </si>
+  <si>
+    <t>User Registration</t>
+  </si>
+  <si>
+    <t>Form for reistration with name last name, email and password. Add to the database the ew user.</t>
+  </si>
+  <si>
+    <t>T35</t>
+  </si>
+  <si>
+    <t>Report Problem System</t>
+  </si>
+  <si>
+    <t>Form with type of question, and a descrition section. When submited it should be attached the client ID and the name of the user.</t>
+  </si>
+  <si>
+    <t>T36</t>
+  </si>
+  <si>
+    <t>Set Profile</t>
+  </si>
+  <si>
+    <t>Add a image to the account. Also, define the addres of the user</t>
+  </si>
+  <si>
+    <t>T37</t>
+  </si>
+  <si>
+    <t>Update Profile</t>
+  </si>
+  <si>
+    <t>Form whereit should be possible to change the password, adress and image</t>
+  </si>
+  <si>
+    <t>T38</t>
+  </si>
+  <si>
+    <t>My Orders Section</t>
+  </si>
+  <si>
+    <t>List the orders that the user already had</t>
+  </si>
+  <si>
+    <t>T39</t>
+  </si>
+  <si>
+    <t>Description of Order Section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show the product list of the order that user seected </t>
+  </si>
+  <si>
+    <t>T40</t>
+  </si>
+  <si>
+    <t>T41</t>
+  </si>
+  <si>
+    <t>Contact Us Page</t>
+  </si>
+  <si>
+    <t>T42</t>
+  </si>
+  <si>
+    <t>Form to send message Section</t>
+  </si>
+  <si>
+    <t>Form with name, email, and description area.</t>
+  </si>
+  <si>
+    <t>T43</t>
+  </si>
+  <si>
+    <t>Formal contacts Section with map</t>
+  </si>
+  <si>
+    <t>Map with the address of the store. Email and phone of the store</t>
+  </si>
+  <si>
+    <t>T44</t>
+  </si>
+  <si>
+    <t>T45</t>
+  </si>
+  <si>
+    <t>Testing and fix some bugs</t>
+  </si>
+  <si>
+    <t>Testing Shopping Cart</t>
+  </si>
+  <si>
+    <t>Test if we the product selected is in the shopping cart. Check if the shopping cart is the same when I log in in a different enviroment</t>
+  </si>
+  <si>
+    <t>T46</t>
+  </si>
+  <si>
+    <t>Search Form, Sorting, Filtering, Pagination</t>
+  </si>
+  <si>
+    <t>Test if the Full Text Searching is working as it should be</t>
+  </si>
+  <si>
+    <t>T47</t>
+  </si>
+  <si>
+    <t>Create account and Login Test</t>
+  </si>
+  <si>
+    <t>Create account, and see if it is succefully loged in. Also check if we restart the browser we need to log in again</t>
+  </si>
+  <si>
+    <t>T48</t>
+  </si>
+  <si>
+    <t>Payments</t>
+  </si>
+  <si>
+    <t>Check if the payment section knows if the payment is already done</t>
+  </si>
+  <si>
+    <t>T49</t>
+  </si>
+  <si>
+    <t>Post Purchase Test</t>
+  </si>
+  <si>
+    <t>Check if user can purchase products.</t>
+  </si>
+  <si>
+    <t>T50</t>
+  </si>
+  <si>
+    <t>Go Live / Deployment</t>
+  </si>
+  <si>
+    <t>Prepare server to receive a bigger amount of requests and lauch a version of the product</t>
+  </si>
+  <si>
+    <t>Total Time:</t>
+  </si>
+  <si>
+    <t>Tasks #</t>
+  </si>
+  <si>
+    <t>17D + 113H</t>
+  </si>
+  <si>
+    <t>113H =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">113 = </t>
+  </si>
+  <si>
+    <t>~18D</t>
+  </si>
+  <si>
+    <t>Estimated time for 5 people:</t>
+  </si>
+  <si>
+    <t>Time to Finish:</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>Assigne</t>
+  </si>
+  <si>
+    <t>No. of Tasks</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Type of Tasks</t>
+  </si>
+  <si>
     <t>Bugs</t>
-  </si>
-  <si>
-    <t>Categories as contact us, sitemap</t>
-  </si>
-  <si>
-    <t>High</t>
-  </si>
-  <si>
-    <t>T9</t>
-  </si>
-  <si>
-    <t>T10</t>
-  </si>
-  <si>
-    <t>Product Page</t>
-  </si>
-  <si>
-    <t>Filtering Option / Serach Product</t>
-  </si>
-  <si>
-    <t>Marina Camilo</t>
-  </si>
-  <si>
-    <t>Full Text Search Database Products</t>
-  </si>
-  <si>
-    <t>T11</t>
-  </si>
-  <si>
-    <t>Top Selling Produc Slider</t>
-  </si>
-  <si>
-    <t>Victor Padi</t>
-  </si>
-  <si>
-    <t>Top Selling Products carousel</t>
-  </si>
-  <si>
-    <t>T12</t>
-  </si>
-  <si>
-    <t>Product Category Section</t>
-  </si>
-  <si>
-    <t>Task</t>
-  </si>
-  <si>
-    <t>Products' miniatures, adjusted by the page dimensions</t>
-  </si>
-  <si>
-    <t>T13</t>
-  </si>
-  <si>
-    <t>T14</t>
-  </si>
-  <si>
-    <t>About Product Page</t>
-  </si>
-  <si>
-    <t>Product Descriptoin Section</t>
-  </si>
-  <si>
-    <t>Section where people can get more info about the product. How is it works? When is it recommend? How should be used? Components and benefits</t>
-  </si>
-  <si>
-    <t>T15</t>
-  </si>
-  <si>
-    <t>Buying Option / Add to cart section</t>
-  </si>
-  <si>
-    <t>Make sure that when you open a new page the cart is the same. If anyone is log in, it keeps the card until the user drops it. Make sure that when a product is selected is on the shopping card section. It has to be possible to change the quantity of a product</t>
-  </si>
-  <si>
-    <t>T16</t>
-  </si>
-  <si>
-    <t>Checkout and payment page</t>
-  </si>
-  <si>
-    <t>Get the total cost of the items of the cart in different coins. Confirm Deliver adress. Check the payment method.</t>
-  </si>
-  <si>
-    <t>T18</t>
-  </si>
-  <si>
-    <t>Blog page</t>
-  </si>
-  <si>
-    <t>Do a comment, change and delete user's loged in comments. See comments from other users, comment others users posts, give reactions to others user posts.</t>
-  </si>
-  <si>
-    <t>T20</t>
-  </si>
-  <si>
-    <t>Events page</t>
-  </si>
-  <si>
-    <t>Creat, update and delete admin's events. See next evets.</t>
-  </si>
-  <si>
-    <t>T21</t>
-  </si>
-  <si>
-    <t>Ecommerce Features</t>
-  </si>
-  <si>
-    <t>Inventory Management</t>
-  </si>
-  <si>
-    <t>Check stock in the store. Know the last bought products and their destiny. See statics of the goods sold. Control the stock requests. Annswer the question of the clients</t>
-  </si>
-  <si>
-    <t>T22</t>
-  </si>
-  <si>
-    <t>Payment Getway integration</t>
-  </si>
-  <si>
-    <t>Conect to the payment portal. Check when the payment is done in the portal.</t>
-  </si>
-  <si>
-    <t>T23</t>
-  </si>
-  <si>
-    <t>Confirmation and Shipment</t>
-  </si>
-  <si>
-    <t>Update the status order.</t>
-  </si>
-  <si>
-    <t>T24</t>
-  </si>
-  <si>
-    <t>Coupons and offers implementation</t>
-  </si>
-  <si>
-    <t>Generate unique numbers of coupons. Create a section to receive any coupon or offer. Check the validation of the coupon/offer</t>
-  </si>
-  <si>
-    <t>T25</t>
-  </si>
-  <si>
-    <t>T26</t>
-  </si>
-  <si>
-    <t>Admin Panel</t>
-  </si>
-  <si>
-    <t>Admin Login and Registration</t>
-  </si>
-  <si>
-    <t>Login should be visible during the site movimentation. Form for registration with name, last name, email and password. Add to the database the ew user.</t>
-  </si>
-  <si>
-    <t>T27</t>
-  </si>
-  <si>
-    <t>Product Upload implementation</t>
-  </si>
-  <si>
-    <t>Form with description, image, cost, and extra information sections. Add to the database the new poduct. It should be visible to users after filling the form</t>
-  </si>
-  <si>
-    <t>T28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Offer and product update </t>
-  </si>
-  <si>
-    <t>Form with description, image, cost, and extra information sections. Update the database about the existing poduct. It should be visible to users after filling the form.</t>
-  </si>
-  <si>
-    <t>T29</t>
-  </si>
-  <si>
-    <t>Admin Logout</t>
-  </si>
-  <si>
-    <t>After closing the browser or click a botton, the admin account should be unacessible</t>
-  </si>
-  <si>
-    <t>T30</t>
-  </si>
-  <si>
-    <t>T31</t>
-  </si>
-  <si>
-    <t>T32</t>
-  </si>
-  <si>
-    <t>User Page</t>
-  </si>
-  <si>
-    <t>T33</t>
-  </si>
-  <si>
-    <t>User Login and Logout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Login should be visible during the site movimentation. Ater click the logout botton or close the browser the user account should be unacessible </t>
-  </si>
-  <si>
-    <t>T34</t>
-  </si>
-  <si>
-    <t>User Registration</t>
-  </si>
-  <si>
-    <t>Form for reistration with name last name, email and password. Add to the database the ew user.</t>
-  </si>
-  <si>
-    <t>T35</t>
-  </si>
-  <si>
-    <t>Report Problem System</t>
-  </si>
-  <si>
-    <t>Form with type of question, and a descrition section. When submited it should be attached the client ID and the name of the user.</t>
-  </si>
-  <si>
-    <t>T36</t>
-  </si>
-  <si>
-    <t>Set Profile</t>
-  </si>
-  <si>
-    <t>Add a image to the account. Also, define the addres of the user</t>
-  </si>
-  <si>
-    <t>T37</t>
-  </si>
-  <si>
-    <t>Update Profile</t>
-  </si>
-  <si>
-    <t>Form whereit should be possible to change the password, adress and image</t>
-  </si>
-  <si>
-    <t>T38</t>
-  </si>
-  <si>
-    <t>My Orders Section</t>
-  </si>
-  <si>
-    <t>List the orders that the user already had</t>
-  </si>
-  <si>
-    <t>T39</t>
-  </si>
-  <si>
-    <t>Description of Order Section</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show the product list of the order that user seected </t>
-  </si>
-  <si>
-    <t>T40</t>
-  </si>
-  <si>
-    <t>T41</t>
-  </si>
-  <si>
-    <t>Contact Us Page</t>
-  </si>
-  <si>
-    <t>T42</t>
-  </si>
-  <si>
-    <t>Form to send message Section</t>
-  </si>
-  <si>
-    <t>Form with name, email, and description area.</t>
-  </si>
-  <si>
-    <t>T43</t>
-  </si>
-  <si>
-    <t>Formal contacts Section with map</t>
-  </si>
-  <si>
-    <t>Map with the address of the store. Email and phone of the store</t>
-  </si>
-  <si>
-    <t>T44</t>
-  </si>
-  <si>
-    <t>T45</t>
-  </si>
-  <si>
-    <t>Testing and fix some bugs</t>
-  </si>
-  <si>
-    <t>Testing Shopping Cart</t>
-  </si>
-  <si>
-    <t>Testing</t>
-  </si>
-  <si>
-    <t>Test if we the product selected is in the shopping cart. Check if the shopping cart is the same when I log in in a different enviroment</t>
-  </si>
-  <si>
-    <t>T46</t>
-  </si>
-  <si>
-    <t>Search Form, Sorting, Filtering, Pagination</t>
-  </si>
-  <si>
-    <t>Test if the Full Text Searching is working as it should be</t>
-  </si>
-  <si>
-    <t>T47</t>
-  </si>
-  <si>
-    <t>Create account and Login Test</t>
-  </si>
-  <si>
-    <t>Create account, and see if it is succefully loged in. Also check if we restart the browser we need to log in again</t>
-  </si>
-  <si>
-    <t>T48</t>
-  </si>
-  <si>
-    <t>Payments</t>
-  </si>
-  <si>
-    <t>Check if the payment section knows if the payment is already done</t>
-  </si>
-  <si>
-    <t>T49</t>
-  </si>
-  <si>
-    <t>Post Purchase Test</t>
-  </si>
-  <si>
-    <t>Check if user can purchase products.</t>
-  </si>
-  <si>
-    <t>T50</t>
-  </si>
-  <si>
-    <t>Go Live / Deployment</t>
-  </si>
-  <si>
-    <t>Prepare server to receive a bigger amount of requests and lauch a version of the product</t>
-  </si>
-  <si>
-    <t>Total Time:</t>
-  </si>
-  <si>
-    <t>Tasks #</t>
-  </si>
-  <si>
-    <t>17D + 113H</t>
-  </si>
-  <si>
-    <t>113H =</t>
-  </si>
-  <si>
-    <t xml:space="preserve">113 = </t>
-  </si>
-  <si>
-    <t>~18D</t>
-  </si>
-  <si>
-    <t>Estimated time for 5 people:</t>
-  </si>
-  <si>
-    <t>Time to Finish:</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>Assigne</t>
-  </si>
-  <si>
-    <t>No. of Tasks</t>
-  </si>
-  <si>
-    <t>Hours</t>
-  </si>
-  <si>
-    <t>Type of Tasks</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="3">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="M/d/yyyy"/>
-    <numFmt numFmtId="165" formatCode="m/d"/>
-    <numFmt numFmtId="166" formatCode="m-d"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -625,23 +722,23 @@
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Roboto Slab"/>
-    </font>
-    <font/>
-    <font>
-      <b/>
     </font>
     <font>
       <b/>
       <sz val="12.0"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Roboto Slab"/>
     </font>
     <font>
       <sz val="11.0"/>
       <color rgb="FF1D2129"/>
       <name val="SFUIText-Regular"/>
+    </font>
+    <font/>
+    <font>
+      <b/>
+      <sz val="12.0"/>
+      <color rgb="FFFFFFFF"/>
     </font>
     <font>
       <color rgb="FF000000"/>
@@ -670,14 +767,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF1155CC"/>
-        <bgColor rgb="FF1155CC"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FF1155CC"/>
+        <bgColor rgb="FF1155CC"/>
       </patternFill>
     </fill>
     <fill>
@@ -699,63 +796,57 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -945,11 +1036,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1305043545"/>
-        <c:axId val="743746004"/>
+        <c:axId val="1679106159"/>
+        <c:axId val="1545273192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1305043545"/>
+        <c:axId val="1679106159"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -981,10 +1072,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="743746004"/>
+        <c:crossAx val="1545273192"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="743746004"/>
+        <c:axId val="1545273192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1015,7 +1106,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1305043545"/>
+        <c:crossAx val="1679106159"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1195,11 +1286,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="2104878673"/>
-        <c:axId val="1367673364"/>
+        <c:axId val="1622712221"/>
+        <c:axId val="757157038"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2104878673"/>
+        <c:axId val="1622712221"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1214,10 +1305,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1367673364"/>
+        <c:crossAx val="757157038"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1367673364"/>
+        <c:axId val="757157038"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1248,7 +1339,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2104878673"/>
+        <c:crossAx val="1622712221"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1264,6 +1355,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1392,10 +1487,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2.0" ySplit="2.0" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="C1" sqref="C1" pane="topRight"/>
+      <pane xSplit="3.0" ySplit="2.0" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="D1" sqref="D1" pane="topRight"/>
       <selection activeCell="A3" sqref="A3" pane="bottomLeft"/>
-      <selection activeCell="C3" sqref="C3" pane="bottomRight"/>
+      <selection activeCell="D3" sqref="D3" pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
@@ -1407,9 +1502,9 @@
     <col customWidth="1" min="6" max="6" width="22.43"/>
     <col customWidth="1" min="7" max="8" width="18.71"/>
     <col customWidth="1" min="9" max="9" width="25.86"/>
-    <col customWidth="1" min="10" max="10" width="27.14"/>
-    <col customWidth="1" hidden="1" min="11" max="11" width="21.14"/>
-    <col customWidth="1" hidden="1" min="12" max="12" width="17.86"/>
+    <col customWidth="1" min="10" max="10" width="24.71"/>
+    <col customWidth="1" min="11" max="11" width="21.14"/>
+    <col customWidth="1" min="12" max="12" width="17.86"/>
     <col customWidth="1" min="13" max="13" width="21.71"/>
     <col customWidth="1" min="14" max="14" width="24.29"/>
     <col customWidth="1" min="15" max="15" width="41.71"/>
@@ -1417,74 +1512,75 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="3" t="s">
+      <c r="D1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>14</v>
+      <c r="E1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6" t="s">
-        <v>15</v>
+      <c r="B2" s="1"/>
+      <c r="C2" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>16</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="J2" s="4"/>
       <c r="L2" s="4" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="D3" s="4">
         <v>16.0</v>
@@ -1492,37 +1588,43 @@
       <c r="E3" s="4">
         <v>5.0</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="H3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="I3" s="8" t="s">
-        <v>23</v>
+        <v>67</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="L3" s="9">
         <v>43047.0</v>
       </c>
-      <c r="M3" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N3" s="4">
-        <v>0.1</v>
+      <c r="M3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="D4" s="4">
         <v>5.0</v>
@@ -1530,38 +1632,41 @@
       <c r="E4" s="4">
         <v>2.0</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>21</v>
+      <c r="F4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="10"/>
+        <v>71</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="K4" s="4" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="L4" s="9">
         <v>43045.0</v>
       </c>
-      <c r="M4" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N4" s="4">
-        <v>0.2</v>
-      </c>
+      <c r="M4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" s="4"/>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="D5" s="4">
         <v>4.0</v>
@@ -1569,49 +1674,51 @@
       <c r="E5" s="4">
         <v>0.0</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>21</v>
+      <c r="F5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5" s="11"/>
+        <v>74</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="K5" s="4" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="L5" s="9">
         <v>43046.0</v>
       </c>
-      <c r="M5" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N5" s="4">
-        <v>0.3</v>
+      <c r="M5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>34</v>
+        <v>75</v>
       </c>
       <c r="F6" s="4"/>
-      <c r="I6" s="12"/>
+      <c r="I6" s="10"/>
       <c r="L6" s="9"/>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>37</v>
+        <v>78</v>
       </c>
       <c r="D7" s="4">
         <v>6.0</v>
@@ -1619,41 +1726,43 @@
       <c r="E7" s="4">
         <v>4.0</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>21</v>
+      <c r="F7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="J7" s="11"/>
+        <v>79</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="K7" s="4" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="L7" s="9">
         <v>43046.0</v>
       </c>
-      <c r="M7" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N7" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="O7" s="13" t="s">
-        <v>39</v>
+      <c r="M7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="O7" s="11" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="D8" s="4">
         <v>8.0</v>
@@ -1661,41 +1770,43 @@
       <c r="E8" s="4">
         <v>2.0</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>21</v>
+      <c r="F8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="J8" s="11"/>
+        <v>83</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="K8" s="4" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="L8" s="9">
         <v>43053.0</v>
       </c>
-      <c r="M8" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N8" s="4">
-        <v>0.3</v>
+      <c r="M8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="O8" s="8" t="s">
-        <v>44</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="D9" s="4">
         <v>5.0</v>
@@ -1703,36 +1814,38 @@
       <c r="E9" s="4">
         <v>1.0</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>21</v>
+      <c r="F9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="J9" s="11"/>
+        <v>87</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="K9" s="4" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="L9" s="9">
         <v>43054.0</v>
       </c>
-      <c r="M9" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N9" s="4">
-        <v>0.3</v>
+      <c r="M9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4"/>
       <c r="C10" s="4" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="D10" s="4">
         <v>5.0</v>
@@ -1740,49 +1853,51 @@
       <c r="E10" s="4">
         <v>2.0</v>
       </c>
-      <c r="F10" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>21</v>
+      <c r="F10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="J10" s="11"/>
+        <v>89</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="K10" s="4" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="L10" s="9">
         <v>43048.0</v>
       </c>
-      <c r="M10" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N10" s="4">
-        <v>0.3</v>
+      <c r="M10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="F11" s="4"/>
-      <c r="I11" s="12"/>
+      <c r="I11" s="10"/>
       <c r="L11" s="9"/>
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>55</v>
+        <v>91</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>92</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>56</v>
+        <v>93</v>
       </c>
       <c r="D12" s="4">
         <v>12.0</v>
@@ -1790,38 +1905,40 @@
       <c r="E12" s="4">
         <v>15.0</v>
       </c>
-      <c r="F12" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>27</v>
+      <c r="F12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="J12" s="11"/>
+        <v>94</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="K12" s="4" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="L12" s="9">
         <v>43048.0</v>
       </c>
-      <c r="M12" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N12" s="4">
-        <v>0.3</v>
+      <c r="M12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>60</v>
+        <v>96</v>
       </c>
       <c r="D13" s="4">
         <v>5.0</v>
@@ -1829,37 +1946,40 @@
       <c r="E13" s="4">
         <v>5.0</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>61</v>
+      <c r="F13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>62</v>
+        <v>97</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="L13" s="9">
         <v>43049.0</v>
       </c>
-      <c r="M13" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N13" s="4">
-        <v>0.3</v>
+      <c r="M13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="D14" s="4">
         <v>8.0</v>
@@ -1867,47 +1987,50 @@
       <c r="E14" s="4">
         <v>8.0</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>61</v>
+      <c r="F14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>66</v>
+        <v>100</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="L14" s="9">
         <v>43052.0</v>
       </c>
-      <c r="M14" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N14" s="4">
-        <v>0.3</v>
+      <c r="M14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="I15" s="12"/>
+        <v>101</v>
+      </c>
+      <c r="I15" s="10"/>
       <c r="L15" s="9"/>
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="D16" s="4">
         <v>4.0</v>
@@ -1915,37 +2038,40 @@
       <c r="E16" s="4">
         <v>4.0</v>
       </c>
-      <c r="F16" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="G16" s="15" t="s">
-        <v>61</v>
+      <c r="F16" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>71</v>
+        <v>105</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="L16" s="9">
         <v>43048.0</v>
       </c>
-      <c r="M16" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N16" s="4">
-        <v>0.3</v>
+      <c r="M16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>73</v>
+        <v>107</v>
       </c>
       <c r="D17" s="4">
         <v>8.0</v>
@@ -1953,37 +2079,40 @@
       <c r="E17" s="4">
         <v>8.0</v>
       </c>
-      <c r="F17" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>61</v>
+      <c r="F17" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>74</v>
+        <v>108</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="L17" s="9">
         <v>43047.0</v>
       </c>
-      <c r="M17" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N17" s="4">
-        <v>0.3</v>
+      <c r="M17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>75</v>
+        <v>109</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="D18" s="4">
         <v>3.0</v>
@@ -1991,29 +2120,32 @@
       <c r="E18" s="4">
         <v>3.0</v>
       </c>
-      <c r="F18" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="G18" s="15" t="s">
-        <v>61</v>
+      <c r="F18" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>77</v>
+        <v>111</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="L18" s="9">
         <v>43048.0</v>
       </c>
-      <c r="M18" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N18" s="4">
-        <v>0.3</v>
+      <c r="M18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="19">
@@ -2022,15 +2154,15 @@
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
-      <c r="I19" s="12"/>
+      <c r="I19" s="10"/>
       <c r="L19" s="9"/>
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
-        <v>78</v>
+        <v>112</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>79</v>
+        <v>113</v>
       </c>
       <c r="D20" s="4">
         <v>8.0</v>
@@ -2039,28 +2171,31 @@
         <v>8.0</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>20</v>
+        <v>31</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>80</v>
+        <v>114</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="L20" s="9">
         <v>43055.0</v>
       </c>
-      <c r="M20" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N20" s="4">
-        <v>0.3</v>
+      <c r="M20" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="21">
@@ -2069,15 +2204,15 @@
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
-      <c r="I21" s="12"/>
+      <c r="I21" s="10"/>
       <c r="L21" s="9"/>
     </row>
     <row r="22">
       <c r="A22" s="4" t="s">
-        <v>81</v>
+        <v>115</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>82</v>
+        <v>116</v>
       </c>
       <c r="D22" s="4">
         <v>8.0</v>
@@ -2085,40 +2220,43 @@
       <c r="E22" s="4">
         <v>8.0</v>
       </c>
-      <c r="F22" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>20</v>
+      <c r="F22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>83</v>
+        <v>117</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="L22" s="9">
         <v>43053.0</v>
       </c>
-      <c r="M22" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N22" s="4">
-        <v>0.3</v>
+      <c r="M22" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="4" t="s">
-        <v>84</v>
+        <v>118</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>85</v>
+        <v>119</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>86</v>
+        <v>120</v>
       </c>
       <c r="D23" s="4">
         <v>16.0</v>
@@ -2126,38 +2264,41 @@
       <c r="E23" s="4">
         <v>16.0</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G23" s="7" t="s">
-        <v>21</v>
-      </c>
       <c r="H23" s="4" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>87</v>
+        <v>121</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="L23" s="9">
         <v>43049.0</v>
       </c>
-      <c r="M23" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N23" s="4">
-        <v>0.3</v>
+      <c r="M23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N23" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="4" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="D24" s="4">
         <v>16.0</v>
@@ -2165,37 +2306,38 @@
       <c r="E24" s="4">
         <v>16.0</v>
       </c>
-      <c r="F24" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G24" s="7" t="s">
+      <c r="F24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H24" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H24" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="I24" s="8" t="s">
-        <v>90</v>
+        <v>124</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="L24" s="9">
         <v>43048.0</v>
       </c>
-      <c r="M24" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N24" s="4">
-        <v>0.3</v>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="4" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="D25" s="4">
         <v>5.0</v>
@@ -2203,37 +2345,40 @@
       <c r="E25" s="4">
         <v>5.0</v>
       </c>
-      <c r="F25" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>20</v>
+      <c r="F25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>93</v>
+        <v>127</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="L25" s="9">
         <v>43046.0</v>
       </c>
-      <c r="M25" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N25" s="4">
-        <v>0.3</v>
+      <c r="M25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N25" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="4" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>95</v>
+        <v>129</v>
       </c>
       <c r="D26" s="4">
         <v>8.0</v>
@@ -2241,48 +2386,51 @@
       <c r="E26" s="4">
         <v>8.0</v>
       </c>
-      <c r="F26" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G26" s="7" t="s">
+      <c r="F26" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="G26" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="H26" s="4" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>96</v>
+        <v>130</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="L26" s="9">
         <v>43054.0</v>
       </c>
-      <c r="M26" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N26" s="4">
-        <v>0.3</v>
+      <c r="M26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N26" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="G27" s="7"/>
-      <c r="I27" s="12"/>
+        <v>131</v>
+      </c>
+      <c r="G27" s="3"/>
+      <c r="I27" s="10"/>
       <c r="L27" s="9"/>
     </row>
     <row r="28">
       <c r="A28" s="4" t="s">
-        <v>98</v>
+        <v>132</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>99</v>
+        <v>133</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>100</v>
+        <v>134</v>
       </c>
       <c r="D28" s="4">
         <v>8.0</v>
@@ -2290,37 +2438,40 @@
       <c r="E28" s="4">
         <v>8.0</v>
       </c>
-      <c r="F28" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>21</v>
+      <c r="F28" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>101</v>
+        <v>135</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="L28" s="9">
         <v>43052.0</v>
       </c>
-      <c r="M28" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N28" s="4">
-        <v>0.3</v>
+      <c r="M28" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N28" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="4" t="s">
-        <v>102</v>
+        <v>136</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>103</v>
+        <v>137</v>
       </c>
       <c r="D29" s="4">
         <v>11.0</v>
@@ -2328,37 +2479,40 @@
       <c r="E29" s="4">
         <v>11.0</v>
       </c>
-      <c r="F29" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>21</v>
+      <c r="F29" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>104</v>
+        <v>138</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="L29" s="9">
         <v>43052.0</v>
       </c>
-      <c r="M29" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N29" s="4">
-        <v>0.3</v>
+      <c r="M29" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N29" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="4" t="s">
-        <v>105</v>
+        <v>139</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>106</v>
+        <v>140</v>
       </c>
       <c r="D30" s="4">
         <v>5.0</v>
@@ -2366,37 +2520,40 @@
       <c r="E30" s="4">
         <v>5.0</v>
       </c>
-      <c r="F30" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>21</v>
+      <c r="F30" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>107</v>
+        <v>141</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="L30" s="9">
         <v>43053.0</v>
       </c>
-      <c r="M30" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N30" s="4">
-        <v>0.3</v>
+      <c r="M30" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N30" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="4" t="s">
-        <v>108</v>
+        <v>142</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="D31" s="4">
         <v>3.0</v>
@@ -2404,61 +2561,64 @@
       <c r="E31" s="4">
         <v>3.0</v>
       </c>
-      <c r="F31" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>20</v>
+      <c r="F31" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>110</v>
+        <v>144</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="L31" s="9">
         <v>43055.0</v>
       </c>
-      <c r="M31" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N31" s="4">
-        <v>0.3</v>
+      <c r="M31" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N31" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="I32" s="12"/>
+        <v>145</v>
+      </c>
+      <c r="I32" s="10"/>
       <c r="L32" s="9"/>
     </row>
     <row r="33">
       <c r="A33" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="I33" s="12"/>
+        <v>146</v>
+      </c>
+      <c r="I33" s="10"/>
       <c r="L33" s="9"/>
     </row>
     <row r="34">
       <c r="A34" s="4" t="s">
-        <v>113</v>
+        <v>147</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="I34" s="12"/>
+        <v>148</v>
+      </c>
+      <c r="I34" s="10"/>
       <c r="L34" s="9"/>
     </row>
     <row r="35">
       <c r="A35" s="4" t="s">
-        <v>115</v>
+        <v>149</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>116</v>
+        <v>150</v>
       </c>
       <c r="D35" s="4">
         <v>4.0</v>
@@ -2466,37 +2626,40 @@
       <c r="E35" s="4">
         <v>4.0</v>
       </c>
-      <c r="F35" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>57</v>
+      <c r="F35" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>117</v>
+        <v>151</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="L35" s="9">
         <v>43049.0</v>
       </c>
-      <c r="M35" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N35" s="4">
-        <v>0.3</v>
+      <c r="M35" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N35" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="4" t="s">
-        <v>118</v>
+        <v>152</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>119</v>
+        <v>153</v>
       </c>
       <c r="D36" s="4">
         <v>6.0</v>
@@ -2504,37 +2667,40 @@
       <c r="E36" s="4">
         <v>6.0</v>
       </c>
-      <c r="F36" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G36" s="7" t="s">
-        <v>57</v>
+      <c r="F36" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>120</v>
+        <v>154</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="L36" s="9">
         <v>43052.0</v>
       </c>
-      <c r="M36" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N36" s="4">
-        <v>0.3</v>
+      <c r="M36" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N36" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="4" t="s">
-        <v>121</v>
+        <v>155</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>122</v>
+        <v>156</v>
       </c>
       <c r="D37" s="4">
         <v>4.0</v>
@@ -2542,37 +2708,40 @@
       <c r="E37" s="4">
         <v>4.0</v>
       </c>
-      <c r="F37" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G37" s="7" t="s">
-        <v>57</v>
+      <c r="F37" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>123</v>
+        <v>157</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="L37" s="9">
         <v>43054.0</v>
       </c>
-      <c r="M37" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N37" s="4">
-        <v>0.3</v>
+      <c r="M37" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N37" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="4" t="s">
-        <v>124</v>
+        <v>158</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>125</v>
+        <v>159</v>
       </c>
       <c r="D38" s="4">
         <v>8.0</v>
@@ -2580,37 +2749,40 @@
       <c r="E38" s="4">
         <v>8.0</v>
       </c>
-      <c r="F38" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G38" s="7" t="s">
-        <v>27</v>
+      <c r="F38" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>126</v>
+        <v>160</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="L38" s="9">
         <v>43052.0</v>
       </c>
-      <c r="M38" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N38" s="4">
-        <v>0.3</v>
+      <c r="M38" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N38" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="4" t="s">
-        <v>127</v>
+        <v>161</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>128</v>
+        <v>162</v>
       </c>
       <c r="D39" s="4">
         <v>4.0</v>
@@ -2618,37 +2790,40 @@
       <c r="E39" s="4">
         <v>4.0</v>
       </c>
-      <c r="F39" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G39" s="7" t="s">
-        <v>27</v>
+      <c r="F39" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>129</v>
+        <v>163</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="L39" s="9">
         <v>43053.0</v>
       </c>
-      <c r="M39" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N39" s="4">
-        <v>0.3</v>
+      <c r="M39" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N39" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="4" t="s">
-        <v>130</v>
+        <v>164</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>131</v>
+        <v>165</v>
       </c>
       <c r="D40" s="4">
         <v>3.0</v>
@@ -2656,38 +2831,41 @@
       <c r="E40" s="4">
         <v>3.0</v>
       </c>
-      <c r="F40" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>20</v>
+      <c r="F40" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>132</v>
+        <v>166</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="L40" s="9">
         <v>43054.0</v>
       </c>
-      <c r="M40" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N40" s="4">
-        <v>0.3</v>
+      <c r="M40" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N40" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="4" t="s">
-        <v>133</v>
+        <v>167</v>
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="4" t="s">
-        <v>134</v>
+        <v>168</v>
       </c>
       <c r="D41" s="4">
         <v>3.0</v>
@@ -2695,54 +2873,57 @@
       <c r="E41" s="4">
         <v>3.0</v>
       </c>
-      <c r="F41" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G41" s="7" t="s">
-        <v>27</v>
+      <c r="F41" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>135</v>
+        <v>169</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="L41" s="9">
         <v>43054.0</v>
       </c>
-      <c r="M41" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N41" s="4">
-        <v>0.3</v>
+      <c r="M41" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N41" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="I42" s="12"/>
+        <v>170</v>
+      </c>
+      <c r="I42" s="10"/>
       <c r="L42" s="9"/>
     </row>
     <row r="43">
       <c r="A43" s="4" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="I43" s="12"/>
+        <v>172</v>
+      </c>
+      <c r="I43" s="10"/>
       <c r="L43" s="9"/>
     </row>
     <row r="44">
       <c r="A44" s="4" t="s">
-        <v>139</v>
+        <v>173</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>140</v>
+        <v>174</v>
       </c>
       <c r="D44" s="4">
         <v>5.0</v>
@@ -2750,37 +2931,40 @@
       <c r="E44" s="4">
         <v>5.0</v>
       </c>
-      <c r="F44" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G44" s="7" t="s">
-        <v>27</v>
+      <c r="F44" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>141</v>
+        <v>175</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="L44" s="9">
         <v>43055.0</v>
       </c>
-      <c r="M44" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N44" s="4">
-        <v>0.3</v>
+      <c r="M44" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N44" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="4" t="s">
-        <v>142</v>
+        <v>176</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>143</v>
+        <v>177</v>
       </c>
       <c r="D45" s="4">
         <v>4.0</v>
@@ -2788,48 +2972,51 @@
       <c r="E45" s="4">
         <v>4.0</v>
       </c>
-      <c r="F45" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G45" s="7" t="s">
-        <v>27</v>
+      <c r="F45" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>144</v>
+        <v>178</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="L45" s="9">
         <v>43047.0</v>
       </c>
-      <c r="M45" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N45" s="4">
-        <v>0.3</v>
+      <c r="M45" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N45" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="I46" s="12"/>
+        <v>179</v>
+      </c>
+      <c r="I46" s="10"/>
       <c r="L46" s="9"/>
       <c r="M46" s="4"/>
     </row>
     <row r="47">
       <c r="A47" s="4" t="s">
-        <v>146</v>
+        <v>180</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>147</v>
+        <v>181</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>148</v>
+        <v>182</v>
       </c>
       <c r="D47" s="4">
         <v>6.0</v>
@@ -2837,37 +3024,40 @@
       <c r="E47" s="4">
         <v>6.0</v>
       </c>
-      <c r="F47" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G47" s="7" t="s">
-        <v>57</v>
+      <c r="F47" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>149</v>
+        <v>26</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>150</v>
+        <v>183</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="K47" s="4" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="L47" s="9">
         <v>43053.0</v>
       </c>
-      <c r="M47" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N47" s="4">
-        <v>0.3</v>
+      <c r="M47" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N47" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="4" t="s">
-        <v>151</v>
+        <v>184</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>152</v>
+        <v>185</v>
       </c>
       <c r="D48" s="4">
         <v>8.0</v>
@@ -2875,37 +3065,40 @@
       <c r="E48" s="4">
         <v>8.0</v>
       </c>
-      <c r="F48" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G48" s="7" t="s">
-        <v>57</v>
+      <c r="F48" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>149</v>
+        <v>26</v>
       </c>
       <c r="I48" s="8" t="s">
-        <v>153</v>
+        <v>186</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="L48" s="9">
         <v>43054.0</v>
       </c>
-      <c r="M48" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N48" s="4">
-        <v>0.3</v>
+      <c r="M48" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N48" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="4" t="s">
-        <v>154</v>
+        <v>187</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>155</v>
+        <v>188</v>
       </c>
       <c r="D49" s="4">
         <v>6.0</v>
@@ -2913,37 +3106,40 @@
       <c r="E49" s="4">
         <v>6.0</v>
       </c>
-      <c r="F49" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="G49" s="7" t="s">
-        <v>27</v>
+      <c r="F49" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>149</v>
+        <v>26</v>
       </c>
       <c r="I49" s="8" t="s">
-        <v>156</v>
+        <v>189</v>
+      </c>
+      <c r="J49" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="L49" s="9">
         <v>43055.0</v>
       </c>
-      <c r="M49" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N49" s="4">
-        <v>0.3</v>
+      <c r="M49" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N49" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="4" t="s">
-        <v>157</v>
+        <v>190</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>158</v>
+        <v>191</v>
       </c>
       <c r="D50" s="4">
         <v>3.0</v>
@@ -2951,37 +3147,40 @@
       <c r="E50" s="4">
         <v>3.0</v>
       </c>
-      <c r="F50" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G50" s="7" t="s">
-        <v>27</v>
+      <c r="F50" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>149</v>
+        <v>26</v>
       </c>
       <c r="I50" s="8" t="s">
-        <v>159</v>
+        <v>192</v>
+      </c>
+      <c r="J50" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="K50" s="4" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="L50" s="9">
         <v>43053.0</v>
       </c>
-      <c r="M50" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N50" s="4">
-        <v>0.3</v>
+      <c r="M50" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N50" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="4" t="s">
-        <v>160</v>
+        <v>193</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>161</v>
+        <v>194</v>
       </c>
       <c r="D51" s="4">
         <v>4.0</v>
@@ -2989,37 +3188,40 @@
       <c r="E51" s="4">
         <v>4.0</v>
       </c>
-      <c r="F51" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G51" s="15" t="s">
-        <v>61</v>
+      <c r="F51" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G51" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>149</v>
+        <v>26</v>
       </c>
       <c r="I51" s="8" t="s">
-        <v>162</v>
+        <v>195</v>
+      </c>
+      <c r="J51" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="K51" s="4" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="L51" s="9">
         <v>43054.0</v>
       </c>
-      <c r="M51" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N51" s="4">
-        <v>0.3</v>
+      <c r="M51" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N51" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="4" t="s">
-        <v>163</v>
+        <v>196</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>164</v>
+        <v>197</v>
       </c>
       <c r="D52" s="4">
         <v>4.0</v>
@@ -3027,29 +3229,32 @@
       <c r="E52" s="4">
         <v>4.0</v>
       </c>
-      <c r="F52" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G52" s="15" t="s">
-        <v>61</v>
+      <c r="F52" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G52" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I52" s="8" t="s">
-        <v>165</v>
+        <v>198</v>
+      </c>
+      <c r="J52" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="K52" s="4" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="L52" s="9">
         <v>43056.0</v>
       </c>
-      <c r="M52" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="N52" s="4">
-        <v>0.3</v>
+      <c r="M52" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N52" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="53">
@@ -3057,51 +3262,161 @@
     </row>
     <row r="55">
       <c r="D55" s="4" t="s">
-        <v>166</v>
+        <v>199</v>
       </c>
     </row>
     <row r="56">
       <c r="B56" s="4" t="s">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>168</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="J56" s="1"/>
     </row>
     <row r="57">
       <c r="B57" s="4">
         <v>38.0</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>169</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="J57" s="4"/>
     </row>
     <row r="58">
       <c r="D58">
         <f>113/6.5</f>
         <v>17.38461538</v>
       </c>
+      <c r="J58" s="4"/>
     </row>
     <row r="59">
       <c r="D59" s="4" t="s">
-        <v>170</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="J59" s="4"/>
     </row>
     <row r="60">
       <c r="D60" s="4" t="s">
-        <v>171</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="J60" s="4"/>
     </row>
     <row r="61">
       <c r="C61" s="4" t="s">
-        <v>172</v>
+        <v>205</v>
       </c>
       <c r="D61">
         <f>35/5</f>
         <v>7</v>
       </c>
+      <c r="J61" s="4"/>
+    </row>
+    <row r="62">
+      <c r="J62" s="4"/>
+    </row>
+    <row r="63">
+      <c r="J63" s="4"/>
+    </row>
+    <row r="64">
+      <c r="J64" s="4"/>
+    </row>
+    <row r="65">
+      <c r="J65" s="4"/>
+    </row>
+    <row r="66">
+      <c r="J66" s="4"/>
+    </row>
+    <row r="67">
+      <c r="J67" s="4"/>
+    </row>
+    <row r="68">
+      <c r="J68" s="4"/>
+    </row>
+    <row r="69">
+      <c r="J69" s="4"/>
+    </row>
+    <row r="70">
+      <c r="J70" s="4"/>
+    </row>
+    <row r="71">
+      <c r="J71" s="4"/>
+    </row>
+    <row r="72">
+      <c r="J72" s="4"/>
+    </row>
+    <row r="73">
+      <c r="J73" s="4"/>
+    </row>
+    <row r="74">
+      <c r="J74" s="4"/>
+    </row>
+    <row r="75">
+      <c r="J75" s="4"/>
+    </row>
+    <row r="76">
+      <c r="J76" s="4"/>
+    </row>
+    <row r="77">
+      <c r="J77" s="4"/>
+    </row>
+    <row r="78">
+      <c r="J78" s="4"/>
+    </row>
+    <row r="79">
+      <c r="J79" s="4"/>
+    </row>
+    <row r="85">
+      <c r="J85" s="4"/>
+    </row>
+    <row r="89">
+      <c r="J89" s="4"/>
     </row>
   </sheetData>
+  <dataValidations>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F3:G52">
+      <formula1>'Dropdown Lists'!$A$2:$A$10</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="M3:M52">
+      <formula1>'Dropdown Lists'!$E$2:$E$30</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="K3:K52">
+      <formula1>'Dropdown Lists'!$D$2:$D$21</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J3:J52">
+      <formula1>'Dropdown Lists'!$C$2:$C$21</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="N3:N52">
+      <formula1>'Dropdown Lists'!$F$2:$F$22</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H3:H52">
+      <formula1>'Dropdown Lists'!$B$2:$B$40</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="J2">
+      <formula1>"Data Base
+Backend
+Home Page,Data Base
+Home Page,Blog Page
+Home Page
+Produtos Page,Data Base
+Product Page,Shopping
+Blog Page,Data Base
+Events,Data Base
+Backend
+Backend,Shopping
+Admin,Data Base
+Admin
+User,Data Base
+User,Shopping
+User,Data Base,Shopping
+Cont"&amp;"act Us
+Shopping
+Data Base
+Admin,User
+Backend,Shopping
+Deployment"</formula1>
+    </dataValidation>
+  </dataValidations>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>
@@ -3114,189 +3429,399 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
+    <col customWidth="1" min="1" max="1" width="15.14"/>
+    <col customWidth="1" min="2" max="2" width="16.14"/>
+    <col customWidth="1" min="3" max="3" width="22.57"/>
+    <col customWidth="1" min="4" max="4" width="15.29"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3"/>
+      <c r="B8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="C11" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="C12" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="C13" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="C14" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="C15" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="C16" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="C17" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="C18" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="C19" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="C20" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="C21" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="C22" s="4"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
     <col customWidth="1" min="1" max="1" width="15.43"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>173</v>
+        <v>206</v>
       </c>
       <c r="B1">
         <f>sum(Sheet1!D3:D52)</f>
         <v>249</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>174</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="16" t="s">
-        <v>5</v>
+      <c r="A2" s="14" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="18">
+      <c r="A3" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="16">
         <f>COUNTIF(Sheet1!$G$3:$G$52,A3)</f>
         <v>8</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" s="18">
+      <c r="A4" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="16">
         <f>COUNTIF(Sheet1!$G$3:$G$52,A4)</f>
         <v>7</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="18">
+      <c r="A5" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="16">
         <f>COUNTIF(Sheet1!$G$3:$G$52,A5)</f>
         <v>6</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="18">
+      <c r="A6" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="16">
         <f>COUNTIF(Sheet1!$G$3:$G$52,A6)</f>
         <v>12</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7" s="18">
+      <c r="A7" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="16">
         <f>COUNTIF(Sheet1!$G$3:$G$52,A7)</f>
         <v>5</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="16" t="s">
-        <v>175</v>
+      <c r="A9" s="14" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="19"/>
-      <c r="B10" s="19" t="s">
-        <v>176</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>177</v>
+      <c r="A10" s="17"/>
+      <c r="B10" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="18">
+      <c r="A11" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="16">
         <f>COUNTIF(Sheet1!$F$3:$F$52,A11)</f>
         <v>8</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="15">
         <f>SUMIF(Sheet1!$F$3:$F$52,A11,Sheet1!$D$3:$D$52)</f>
         <v>51</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" s="18">
+      <c r="A12" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="16">
         <f>COUNTIF(Sheet1!$F$3:$F$52,A12)</f>
         <v>8</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C12" s="15">
         <f>SUMIF(Sheet1!$F$3:$F$52,A12,Sheet1!$D$3:$D$52)</f>
         <v>48</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="18">
+      <c r="A13" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="16">
         <f>COUNTIF(Sheet1!$F$3:$F$52,A13)</f>
         <v>6</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="15">
         <f>SUMIF(Sheet1!$F$3:$F$52,A13,Sheet1!$D$3:$D$52)</f>
         <v>50</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="18">
+      <c r="A14" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="16">
         <f>COUNTIF(Sheet1!$F$3:$F$52,A14)</f>
         <v>9</v>
       </c>
-      <c r="C14" s="17">
+      <c r="C14" s="15">
         <f>SUMIF(Sheet1!$F$3:$F$52,A14,Sheet1!$D$3:$D$52)</f>
         <v>52</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="B15" s="18">
+      <c r="A15" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="16">
         <f>COUNTIF(Sheet1!$F$3:$F$52,A15)</f>
         <v>7</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C15" s="15">
         <f>SUMIF(Sheet1!$F$3:$F$52,A15,Sheet1!$D$3:$D$52)</f>
         <v>48</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="16" t="s">
-        <v>178</v>
+      <c r="A17" s="14" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" s="18">
+      <c r="A18" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="B18" s="16">
         <f>COUNTIF(Sheet1!$H$3:$H$52,A18)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="18">
+      <c r="A19" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="16">
         <f>COUNTIF(Sheet1!$H$3:$H$52,A19)</f>
         <v>2</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="18">
+      <c r="A20" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="16">
         <f>COUNTIF(Sheet1!$H$3:$H$52,A20)</f>
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="B21" s="18">
+      <c r="A21" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="16">
         <f>COUNTIF(Sheet1!$H$3:$H$52,A21)</f>
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23">

</xml_diff>